<commit_message>
Remove data in TextPropToScript of tax_calc_no_glob
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/mapping/accounton_mapping.xlsx
+++ b/excel_tax_calculation/mapping/accounton_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/codebases/pit-tax-calculation/excel_tax_calculation/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA54E630-1A20-0643-89BB-40F8ED8755C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1B9CF0-B8B4-AE4F-B52D-10BC4E507B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="19500" xr2:uid="{3B2B5E63-447A-5843-B8A1-1A316823146C}"/>
   </bookViews>
@@ -9261,7 +9261,7 @@
   <dimension ref="A1:H1034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A927" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A928" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D965" sqref="D965:D966"/>
     </sheetView>
   </sheetViews>

</xml_diff>